<commit_message>
Ny oppdatering oktober 2022
</commit_message>
<xml_diff>
--- a/data til pbi/LineName.xlsx
+++ b/data til pbi/LineName.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeidsprosjekter\Github - VTpluss\Bypakke Grenland\bypakke_grenland\data til pbi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeidsområde\github\bypakke_grenland\data til pbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E9385A-DFEB-48D3-9444-1AF878D20CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CA92F3-3BED-4D19-A924-77DAB73E5A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46656" yWindow="-108" windowWidth="23040" windowHeight="12216" xr2:uid="{AA9D0BA4-9C0C-4CA4-B340-2A57C39C49F5}"/>
+    <workbookView xWindow="3324" yWindow="636" windowWidth="26628" windowHeight="15804" xr2:uid="{AA9D0BA4-9C0C-4CA4-B340-2A57C39C49F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>PublicLineNo</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Skien-Bølehøgda-Porsgrunn-Herre</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>Gulset-Porsgrunn</t>
   </si>
 </sst>
 </file>
@@ -571,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117C6572-4F76-4820-AC76-49A7FBA3DEBB}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,288 +688,299 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>70</v>
+      <c r="A10" t="s">
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C10">
-        <v>8070</v>
+        <v>8010</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>8084</v>
+        <v>8070</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>281</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C12">
-        <v>8281</v>
+        <v>8084</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>710</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>8710</v>
+        <v>8281</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>8711</v>
+        <v>8710</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
+        <v>711</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>8711</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>712</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>8712</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16">
-        <v>8801</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17">
-        <v>8802</v>
+        <v>8801</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18">
-        <v>8803</v>
+        <v>8802</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19">
-        <v>8804</v>
+        <v>8803</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20">
-        <v>8805</v>
+        <v>8804</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C21">
-        <v>8806</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C22">
-        <v>8807</v>
+        <v>8806</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C23">
-        <v>8810</v>
+        <v>8807</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>8811</v>
+        <v>8810</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25">
-        <v>8812</v>
+        <v>8811</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26">
-        <v>8813</v>
+        <v>8812</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27">
-        <v>8814</v>
+        <v>8813</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28">
-        <v>8815</v>
+        <v>8814</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29">
-        <v>8816</v>
+        <v>8815</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30">
-        <v>8817</v>
+        <v>8816</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31">
-        <v>8818</v>
+        <v>8817</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32">
-        <v>8819</v>
+        <v>8818</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33">
+        <v>8819</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>54</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>55</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>8820</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>81</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34">
-        <v>8881</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35">
+        <v>8881</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>82</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>57</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>8882</v>
       </c>
     </row>

</xml_diff>